<commit_message>
importer field name error
</commit_message>
<xml_diff>
--- a/sample_data/41612_2019_62_MOESM2_ESM_simplified.xlsx
+++ b/sample_data/41612_2019_62_MOESM2_ESM_simplified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeshan/Documents/github/sparrow-uw-cosmo/sample_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92060F94-849F-CE42-B32D-4B4260C78D03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCE69F3-0FEC-8443-8905-B88BD6E599D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="460" windowWidth="26780" windowHeight="17460" tabRatio="936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="500" windowWidth="26780" windowHeight="17460" tabRatio="936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRONUS_input" sheetId="19" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="170">
   <si>
     <t>SBO-SFF-07</t>
   </si>
@@ -607,6 +607,12 @@
   <si>
     <t>test</t>
   </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Atm-Pressure</t>
+  </si>
 </sst>
 </file>
 
@@ -1707,7 +1713,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1734,6 +1740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1027">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3492,10 +3499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5AE1AF7-AA38-4C4B-A483-9105C007B640}">
-  <dimension ref="A1:S136"/>
+  <dimension ref="A1:T136"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3503,7 +3510,7 @@
     <col min="6" max="6" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>62</v>
       </c>
@@ -3561,8 +3568,11 @@
       <c r="S1" s="10" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" ht="14" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="T1" s="10" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="14" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11"/>
       <c r="B2" s="11">
         <v>1</v>
@@ -3612,14 +3622,17 @@
       <c r="Q2" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="R2">
-        <v>1001</v>
-      </c>
-      <c r="S2">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="R2" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S2" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -3665,10 +3678,23 @@
       <c r="O3" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R3" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S3" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>64</v>
       </c>
@@ -3714,8 +3740,23 @@
       <c r="O4" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R4" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S4" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>65</v>
       </c>
@@ -3761,8 +3802,23 @@
       <c r="O5" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R5" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S5" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
@@ -3808,8 +3864,23 @@
       <c r="O6" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R6" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S6" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>67</v>
       </c>
@@ -3855,8 +3926,23 @@
       <c r="O7" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R7" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S7" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -3902,8 +3988,23 @@
       <c r="O8" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R8" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S8" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>69</v>
       </c>
@@ -3949,8 +4050,23 @@
       <c r="O9" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R9" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S9" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
@@ -3996,8 +4112,23 @@
       <c r="O10" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R10" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S10" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>71</v>
       </c>
@@ -4043,8 +4174,23 @@
       <c r="O11" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R11" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S11" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
@@ -4090,8 +4236,23 @@
       <c r="O12" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R12" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S12" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>73</v>
       </c>
@@ -4137,8 +4298,23 @@
       <c r="O13" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R13" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S13" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>74</v>
       </c>
@@ -4184,8 +4360,23 @@
       <c r="O14" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R14" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S14" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -4231,8 +4422,23 @@
       <c r="O15" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="P15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R15" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S15" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -4278,8 +4484,23 @@
       <c r="O16" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P16" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R16" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S16" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>77</v>
       </c>
@@ -4325,8 +4546,23 @@
       <c r="O17" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R17" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S17" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>78</v>
       </c>
@@ -4372,8 +4608,23 @@
       <c r="O18" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R18" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S18" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
@@ -4419,8 +4670,23 @@
       <c r="O19" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R19" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S19" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>117</v>
       </c>
@@ -4466,8 +4732,23 @@
       <c r="O20" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R20" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S20" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>118</v>
       </c>
@@ -4513,8 +4794,23 @@
       <c r="O21" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R21" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S21" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>119</v>
       </c>
@@ -4560,8 +4856,23 @@
       <c r="O22" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R22" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S22" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>120</v>
       </c>
@@ -4607,8 +4918,23 @@
       <c r="O23" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R23" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S23" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>121</v>
       </c>
@@ -4654,8 +4980,23 @@
       <c r="O24" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R24" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S24" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>122</v>
       </c>
@@ -4701,8 +5042,23 @@
       <c r="O25" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R25" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S25" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -4748,8 +5104,23 @@
       <c r="O26" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P26" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R26" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S26" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>69</v>
       </c>
@@ -4795,8 +5166,23 @@
       <c r="O27" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R27" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S27" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
@@ -4842,8 +5228,23 @@
       <c r="O28" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R28" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S28" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
@@ -4889,8 +5290,23 @@
       <c r="O29" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R29" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S29" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -4936,8 +5352,23 @@
       <c r="O30" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R30" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S30" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -4983,8 +5414,23 @@
       <c r="O31" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R31" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S31" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -5030,8 +5476,23 @@
       <c r="O32" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R32" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S32" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>6</v>
       </c>
@@ -5077,8 +5538,23 @@
       <c r="O33" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R33" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S33" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>7</v>
       </c>
@@ -5124,8 +5600,23 @@
       <c r="O34" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R34" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S34" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -5171,8 +5662,23 @@
       <c r="O35" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R35" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S35" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -5218,8 +5724,23 @@
       <c r="O36" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P36" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R36" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S36" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -5265,8 +5786,23 @@
       <c r="O37" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R37" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S37" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>11</v>
       </c>
@@ -5312,8 +5848,23 @@
       <c r="O38" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P38" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R38" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S38" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -5359,8 +5910,23 @@
       <c r="O39" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R39" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S39" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
@@ -5406,8 +5972,23 @@
       <c r="O40" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P40" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R40" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S40" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -5453,8 +6034,23 @@
       <c r="O41" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P41" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R41" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S41" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>15</v>
       </c>
@@ -5500,8 +6096,23 @@
       <c r="O42" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P42" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q42" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R42" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S42" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>16</v>
       </c>
@@ -5547,8 +6158,23 @@
       <c r="O43" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R43" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S43" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>17</v>
       </c>
@@ -5594,8 +6220,23 @@
       <c r="O44" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P44" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R44" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S44" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>18</v>
       </c>
@@ -5641,8 +6282,23 @@
       <c r="O45" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q45" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R45" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S45" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>69</v>
       </c>
@@ -5688,8 +6344,23 @@
       <c r="O46" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q46" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R46" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S46" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
@@ -5735,8 +6406,23 @@
       <c r="O47" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q47" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R47" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S47" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>69</v>
       </c>
@@ -5782,8 +6468,23 @@
       <c r="O48" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q48" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R48" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S48" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>19</v>
       </c>
@@ -5829,8 +6530,23 @@
       <c r="O49" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q49" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R49" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S49" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
@@ -5876,8 +6592,23 @@
       <c r="O50" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P50" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q50" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R50" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S50" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
         <v>21</v>
       </c>
@@ -5923,8 +6654,23 @@
       <c r="O51" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R51" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S51" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>22</v>
       </c>
@@ -5970,8 +6716,23 @@
       <c r="O52" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P52" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q52" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R52" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S52" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
         <v>23</v>
       </c>
@@ -6017,8 +6778,23 @@
       <c r="O53" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R53" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S53" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>24</v>
       </c>
@@ -6064,8 +6840,23 @@
       <c r="O54" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P54" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q54" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R54" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S54" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>25</v>
       </c>
@@ -6111,8 +6902,23 @@
       <c r="O55" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P55" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q55" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R55" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S55" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>26</v>
       </c>
@@ -6158,8 +6964,23 @@
       <c r="O56" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P56" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q56" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R56" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S56" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
         <v>27</v>
       </c>
@@ -6205,8 +7026,23 @@
       <c r="O57" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R57" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S57" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
         <v>28</v>
       </c>
@@ -6252,8 +7088,23 @@
       <c r="O58" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P58" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q58" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R58" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S58" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
         <v>29</v>
       </c>
@@ -6299,8 +7150,23 @@
       <c r="O59" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R59" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S59" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
         <v>30</v>
       </c>
@@ -6346,8 +7212,23 @@
       <c r="O60" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P60" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q60" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R60" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S60" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
         <v>31</v>
       </c>
@@ -6393,8 +7274,23 @@
       <c r="O61" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R61" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S61" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
         <v>32</v>
       </c>
@@ -6440,8 +7336,23 @@
       <c r="O62" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R62" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S62" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
@@ -6487,8 +7398,23 @@
       <c r="O63" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P63" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q63" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R63" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S63" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
         <v>34</v>
       </c>
@@ -6534,8 +7460,23 @@
       <c r="O64" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P64" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R64" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S64" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>35</v>
       </c>
@@ -6581,8 +7522,23 @@
       <c r="O65" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P65" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q65" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R65" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S65" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>36</v>
       </c>
@@ -6628,8 +7584,23 @@
       <c r="O66" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q66" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R66" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S66" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
         <v>37</v>
       </c>
@@ -6675,8 +7646,23 @@
       <c r="O67" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P67" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R67" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S67" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
         <v>38</v>
       </c>
@@ -6722,8 +7708,23 @@
       <c r="O68" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P68" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q68" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R68" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S68" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
         <v>39</v>
       </c>
@@ -6769,8 +7770,23 @@
       <c r="O69" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P69" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q69" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R69" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S69" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
         <v>40</v>
       </c>
@@ -6816,8 +7832,23 @@
       <c r="O70" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R70" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S70" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>41</v>
       </c>
@@ -6863,8 +7894,23 @@
       <c r="O71" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R71" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S71" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>42</v>
       </c>
@@ -6910,8 +7956,23 @@
       <c r="O72" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R72" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S72" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>43</v>
       </c>
@@ -6957,8 +8018,23 @@
       <c r="O73" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R73" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S73" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
         <v>44</v>
       </c>
@@ -7004,8 +8080,23 @@
       <c r="O74" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R74" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S74" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
         <v>45</v>
       </c>
@@ -7051,8 +8142,23 @@
       <c r="O75" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R75" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S75" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
         <v>46</v>
       </c>
@@ -7098,8 +8204,23 @@
       <c r="O76" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P76" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R76" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S76" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
         <v>47</v>
       </c>
@@ -7145,8 +8266,23 @@
       <c r="O77" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P77" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R77" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S77" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
         <v>48</v>
       </c>
@@ -7192,8 +8328,23 @@
       <c r="O78" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P78" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R78" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S78" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>49</v>
       </c>
@@ -7239,8 +8390,23 @@
       <c r="O79" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P79" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R79" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S79" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>50</v>
       </c>
@@ -7286,8 +8452,23 @@
       <c r="O80" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P80" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q80" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R80" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S80" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>51</v>
       </c>
@@ -7333,8 +8514,23 @@
       <c r="O81" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R81" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S81" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
         <v>52</v>
       </c>
@@ -7380,8 +8576,23 @@
       <c r="O82" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q82" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R82" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S82" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
         <v>53</v>
       </c>
@@ -7427,8 +8638,23 @@
       <c r="O83" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P83" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R83" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S83" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
         <v>54</v>
       </c>
@@ -7474,8 +8700,23 @@
       <c r="O84" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P84" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q84" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R84" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S84" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
         <v>55</v>
       </c>
@@ -7521,8 +8762,23 @@
       <c r="O85" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R85" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S85" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>56</v>
       </c>
@@ -7568,8 +8824,23 @@
       <c r="O86" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P86" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q86" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R86" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S86" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>57</v>
       </c>
@@ -7615,8 +8886,23 @@
       <c r="O87" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P87" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q87" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R87" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S87" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
         <v>58</v>
       </c>
@@ -7662,8 +8948,23 @@
       <c r="O88" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P88" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q88" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R88" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S88" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
         <v>59</v>
       </c>
@@ -7709,8 +9010,23 @@
       <c r="O89" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q89" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R89" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S89" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
         <v>60</v>
       </c>
@@ -7756,8 +9072,23 @@
       <c r="O90" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P90" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q90" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R90" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S90" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
         <v>61</v>
       </c>
@@ -7803,8 +9134,23 @@
       <c r="O91" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P91" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q91" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R91" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S91" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
         <v>123</v>
       </c>
@@ -7850,8 +9196,23 @@
       <c r="O92" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P92" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q92" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R92" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S92" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>124</v>
       </c>
@@ -7897,8 +9258,23 @@
       <c r="O93" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P93" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q93" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R93" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S93" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>125</v>
       </c>
@@ -7944,8 +9320,23 @@
       <c r="O94" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P94" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q94" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R94" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S94" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
         <v>126</v>
       </c>
@@ -7991,8 +9382,23 @@
       <c r="O95" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P95" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q95" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R95" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S95" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
         <v>127</v>
       </c>
@@ -8038,8 +9444,23 @@
       <c r="O96" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P96" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q96" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R96" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S96" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
         <v>80</v>
       </c>
@@ -8085,8 +9506,23 @@
       <c r="O97" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P97" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q97" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R97" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S97" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
         <v>81</v>
       </c>
@@ -8132,8 +9568,23 @@
       <c r="O98" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P98" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q98" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R98" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S98" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
         <v>82</v>
       </c>
@@ -8179,8 +9630,23 @@
       <c r="O99" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P99" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R99" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S99" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>83</v>
       </c>
@@ -8226,8 +9692,23 @@
       <c r="O100" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P100" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q100" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R100" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S100" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
         <v>84</v>
       </c>
@@ -8273,8 +9754,23 @@
       <c r="O101" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P101" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q101" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R101" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S101" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
         <v>85</v>
       </c>
@@ -8320,8 +9816,23 @@
       <c r="O102" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P102" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q102" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R102" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S102" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
         <v>86</v>
       </c>
@@ -8367,8 +9878,23 @@
       <c r="O103" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P103" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q103" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R103" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S103" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
         <v>87</v>
       </c>
@@ -8414,8 +9940,23 @@
       <c r="O104" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P104" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q104" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R104" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S104" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
         <v>88</v>
       </c>
@@ -8461,8 +10002,23 @@
       <c r="O105" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P105" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q105" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R105" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S105" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
         <v>89</v>
       </c>
@@ -8508,8 +10064,23 @@
       <c r="O106" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P106" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q106" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R106" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S106" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
         <v>90</v>
       </c>
@@ -8555,8 +10126,23 @@
       <c r="O107" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P107" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q107" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R107" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S107" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
         <v>91</v>
       </c>
@@ -8602,8 +10188,23 @@
       <c r="O108" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P108" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R108" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S108" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
         <v>92</v>
       </c>
@@ -8649,8 +10250,23 @@
       <c r="O109" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P109" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q109" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R109" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S109" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
         <v>93</v>
       </c>
@@ -8696,8 +10312,23 @@
       <c r="O110" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P110" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q110" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R110" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S110" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
         <v>94</v>
       </c>
@@ -8743,8 +10374,23 @@
       <c r="O111" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P111" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q111" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R111" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S111" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
         <v>95</v>
       </c>
@@ -8790,8 +10436,23 @@
       <c r="O112" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P112" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q112" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R112" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S112" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
         <v>96</v>
       </c>
@@ -8837,8 +10498,23 @@
       <c r="O113" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P113" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q113" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R113" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S113" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
         <v>97</v>
       </c>
@@ -8884,8 +10560,23 @@
       <c r="O114" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P114" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q114" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R114" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S114" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
         <v>98</v>
       </c>
@@ -8931,8 +10622,23 @@
       <c r="O115" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P115" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q115" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R115" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S115" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
         <v>99</v>
       </c>
@@ -8978,8 +10684,23 @@
       <c r="O116" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P116" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q116" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R116" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S116" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
         <v>100</v>
       </c>
@@ -9025,8 +10746,23 @@
       <c r="O117" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P117" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q117" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R117" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S117" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
         <v>101</v>
       </c>
@@ -9072,8 +10808,23 @@
       <c r="O118" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P118" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q118" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R118" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S118" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
         <v>102</v>
       </c>
@@ -9119,8 +10870,23 @@
       <c r="O119" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q119" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R119" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S119" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
         <v>103</v>
       </c>
@@ -9166,8 +10932,23 @@
       <c r="O120" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P120" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q120" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R120" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S120" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
         <v>104</v>
       </c>
@@ -9213,8 +10994,23 @@
       <c r="O121" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P121" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q121" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R121" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S121" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
         <v>105</v>
       </c>
@@ -9260,8 +11056,23 @@
       <c r="O122" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P122" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q122" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R122" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S122" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
         <v>106</v>
       </c>
@@ -9307,8 +11118,23 @@
       <c r="O123" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P123" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q123" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R123" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S123" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
         <v>107</v>
       </c>
@@ -9354,8 +11180,23 @@
       <c r="O124" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P124" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R124" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S124" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
         <v>69</v>
       </c>
@@ -9401,8 +11242,23 @@
       <c r="O125" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P125" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q125" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R125" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S125" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
         <v>67</v>
       </c>
@@ -9448,8 +11304,23 @@
       <c r="O126" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P126" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q126" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R126" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S126" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
         <v>69</v>
       </c>
@@ -9495,8 +11366,23 @@
       <c r="O127" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q127" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R127" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S127" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
         <v>67</v>
       </c>
@@ -9542,8 +11428,23 @@
       <c r="O128" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P128" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R128" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S128" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
         <v>128</v>
       </c>
@@ -9589,8 +11490,23 @@
       <c r="O129" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q129" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R129" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S129" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
         <v>129</v>
       </c>
@@ -9636,8 +11552,23 @@
       <c r="O130" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P130" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q130" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R130" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S130" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
         <v>130</v>
       </c>
@@ -9683,8 +11614,23 @@
       <c r="O131" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P131" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q131" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R131" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S131" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
         <v>131</v>
       </c>
@@ -9730,8 +11676,23 @@
       <c r="O132" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P132" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q132" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R132" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S132" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
         <v>132</v>
       </c>
@@ -9777,8 +11738,23 @@
       <c r="O133" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P133" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q133" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R133" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S133" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
         <v>133</v>
       </c>
@@ -9824,8 +11800,23 @@
       <c r="O134" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P134" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q134" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R134" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S134" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
         <v>134</v>
       </c>
@@ -9871,8 +11862,23 @@
       <c r="O135" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="P135" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q135" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R135" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S135" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
         <v>135</v>
       </c>
@@ -9917,6 +11923,21 @@
       </c>
       <c r="O136" s="1" t="s">
         <v>116</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="R136" s="12">
+        <v>35347</v>
+      </c>
+      <c r="S136" s="12">
+        <v>35347</v>
+      </c>
+      <c r="T136">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>